<commit_message>
more environmental stats, and cleaned up and moved sample data file
</commit_message>
<xml_diff>
--- a/data/Survival-stats.xlsx
+++ b/data/Survival-stats.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28331"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="0" windowWidth="11800" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8700" yWindow="0" windowWidth="16900" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2017-08-14-Geoduck-samples.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Summary Stats" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Summary Stats'!$B$1:$E$54</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="1">'Summary Stats'!$J:$L</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Summary Stats'!$B$1:$D$54</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="1">'Summary Stats'!$I:$K</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="256">
   <si>
     <t>Box #</t>
   </si>
@@ -765,6 +766,33 @@
   </si>
   <si>
     <t>Overall % Survival</t>
+  </si>
+  <si>
+    <t>WBB</t>
+  </si>
+  <si>
+    <t>CIB</t>
+  </si>
+  <si>
+    <t>CIE</t>
+  </si>
+  <si>
+    <t>FBB</t>
+  </si>
+  <si>
+    <t>FBE</t>
+  </si>
+  <si>
+    <t>PGB</t>
+  </si>
+  <si>
+    <t>PGE</t>
+  </si>
+  <si>
+    <t>EELGRASS</t>
+  </si>
+  <si>
+    <t>BARE</t>
   </si>
 </sst>
 </file>
@@ -833,9 +861,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -892,7 +940,7 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -908,6 +956,16 @@
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -923,6 +981,16 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1255,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W183"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+    <sheetView topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6923,21 +6991,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24:M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="6" width="10.83203125" style="2"/>
-    <col min="8" max="8" width="10.83203125" style="3"/>
-    <col min="13" max="13" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" style="3" customWidth="1"/>
+    <col min="1" max="5" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="10.83203125" style="3"/>
+    <col min="12" max="12" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" ht="54">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="54">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -6948,40 +7016,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>242</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J1" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -6992,45 +7057,42 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B2,'2017-08-14-Geoduck-samples.csv'!C:C,C2,'2017-08-14-Geoduck-samples.csv'!E:E,E2,'2017-08-14-Geoduck-samples.csv'!F:F,F2)</f>
-        <v>4</v>
-      </c>
-      <c r="H2" s="3">
-        <f>G2/5</f>
+        <v>39</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B2,'2017-08-14-Geoduck-samples.csv'!C:C,C2,'2017-08-14-Geoduck-samples.csv'!E:E,D2,'2017-08-14-Geoduck-samples.csv'!F:F,E2)</f>
+        <v>4</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2/5</f>
         <v>0.8</v>
       </c>
-      <c r="J2" s="8">
-        <v>1</v>
+      <c r="I2" s="8">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
+        <v>39</v>
+      </c>
+      <c r="L2" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
         <v>0.9</v>
       </c>
-      <c r="N2" s="10">
-        <f>SUMIFS(G:G,B:B,J:J,C:C,K:K,E:E,L:L)</f>
+      <c r="M2" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
         <v>9</v>
       </c>
-      <c r="O2" s="9">
-        <f>N2/15</f>
+      <c r="N2" s="9">
+        <f>M2/15</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -7041,45 +7103,42 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="2">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="G3">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B3,'2017-08-14-Geoduck-samples.csv'!C:C,C3,'2017-08-14-Geoduck-samples.csv'!E:E,E3,'2017-08-14-Geoduck-samples.csv'!F:F,F3)</f>
+      <c r="F3">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B3,'2017-08-14-Geoduck-samples.csv'!C:C,C3,'2017-08-14-Geoduck-samples.csv'!E:E,D3,'2017-08-14-Geoduck-samples.csv'!F:F,E3)</f>
         <v>5</v>
       </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H54" si="0">G3/5</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <v>1</v>
+      <c r="G3" s="3">
+        <f>F3/5</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
+        <v>17</v>
+      </c>
+      <c r="L3" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="N3" s="10">
-        <f t="shared" ref="N3:N21" si="1">SUMIFS(G:G,B:B,J:J,C:C,K:K,E:E,L:L)</f>
+      <c r="M3" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
         <v>10</v>
       </c>
-      <c r="O3" s="9">
-        <f>N3/15</f>
+      <c r="N3" s="9">
+        <f>M3/15</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -7090,878 +7149,824 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B4,'2017-08-14-Geoduck-samples.csv'!C:C,C4,'2017-08-14-Geoduck-samples.csv'!E:E,E4,'2017-08-14-Geoduck-samples.csv'!F:F,F4)</f>
-        <v>1</v>
-      </c>
-      <c r="H4" s="3">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B4,'2017-08-14-Geoduck-samples.csv'!C:C,C4,'2017-08-14-Geoduck-samples.csv'!E:E,D4,'2017-08-14-Geoduck-samples.csv'!F:F,E4)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <f>F4/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="M4" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>12</v>
+      </c>
+      <c r="N4" s="9">
+        <f t="shared" ref="N4:N21" si="0">M4/15</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B5,'2017-08-14-Geoduck-samples.csv'!C:C,C5,'2017-08-14-Geoduck-samples.csv'!E:E,D5,'2017-08-14-Geoduck-samples.csv'!F:F,E5)</f>
+        <v>4</v>
+      </c>
+      <c r="G5" s="3">
+        <f>F5/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="M5" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>13</v>
+      </c>
+      <c r="N5" s="9">
+        <f t="shared" si="0"/>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B6,'2017-08-14-Geoduck-samples.csv'!C:C,C6,'2017-08-14-Geoduck-samples.csv'!E:E,D6,'2017-08-14-Geoduck-samples.csv'!F:F,E6)</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="3">
+        <f>F6/5</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.93333333333333324</v>
+      </c>
+      <c r="M6" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>14</v>
+      </c>
+      <c r="N6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B7,'2017-08-14-Geoduck-samples.csv'!C:C,C7,'2017-08-14-Geoduck-samples.csv'!E:E,D7,'2017-08-14-Geoduck-samples.csv'!F:F,E7)</f>
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="M7" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>12</v>
+      </c>
+      <c r="N7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B8,'2017-08-14-Geoduck-samples.csv'!C:C,C8,'2017-08-14-Geoduck-samples.csv'!E:E,D8,'2017-08-14-Geoduck-samples.csv'!F:F,E8)</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <f>F8/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M8" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>2</v>
+      </c>
+      <c r="N8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B9,'2017-08-14-Geoduck-samples.csv'!C:C,C9,'2017-08-14-Geoduck-samples.csv'!E:E,D9,'2017-08-14-Geoduck-samples.csv'!F:F,E9)</f>
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
+        <f>F9/5</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="M9" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>11</v>
+      </c>
+      <c r="N9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B10,'2017-08-14-Geoduck-samples.csv'!C:C,C10,'2017-08-14-Geoduck-samples.csv'!E:E,D10,'2017-08-14-Geoduck-samples.csv'!F:F,E10)</f>
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <f>F10/5</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>1</v>
+      </c>
+      <c r="M10" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>15</v>
+      </c>
+      <c r="N10" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B11,'2017-08-14-Geoduck-samples.csv'!C:C,C11,'2017-08-14-Geoduck-samples.csv'!E:E,D11,'2017-08-14-Geoduck-samples.csv'!F:F,E11)</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="3">
+        <f>F11/5</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="9">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.93333333333333324</v>
+      </c>
+      <c r="M11" s="10">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>14</v>
+      </c>
+      <c r="N11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B12,'2017-08-14-Geoduck-samples.csv'!C:C,C12,'2017-08-14-Geoduck-samples.csv'!E:E,D12,'2017-08-14-Geoduck-samples.csv'!F:F,E12)</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
+        <f>F12/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="M12">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>6</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B13,'2017-08-14-Geoduck-samples.csv'!C:C,C13,'2017-08-14-Geoduck-samples.csv'!E:E,D13,'2017-08-14-Geoduck-samples.csv'!F:F,E13)</f>
+        <v>5</v>
+      </c>
+      <c r="G13" s="3">
+        <f>F13/5</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.46666666666666662</v>
+      </c>
+      <c r="M13">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>7</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B14,'2017-08-14-Geoduck-samples.csv'!C:C,C14,'2017-08-14-Geoduck-samples.csv'!E:E,D14,'2017-08-14-Geoduck-samples.csv'!F:F,E14)</f>
+        <v>4</v>
+      </c>
+      <c r="G14" s="3">
+        <f>F14/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.9</v>
+      </c>
+      <c r="M14">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>9</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B15,'2017-08-14-Geoduck-samples.csv'!C:C,C15,'2017-08-14-Geoduck-samples.csv'!E:E,D15,'2017-08-14-Geoduck-samples.csv'!F:F,E15)</f>
+        <v>5</v>
+      </c>
+      <c r="G15" s="3">
+        <f>F15/5</f>
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M15">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>6</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B16,'2017-08-14-Geoduck-samples.csv'!C:C,C16,'2017-08-14-Geoduck-samples.csv'!E:E,D16,'2017-08-14-Geoduck-samples.csv'!F:F,E16)</f>
+        <v>3</v>
+      </c>
+      <c r="G16" s="3">
+        <f>F16/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M16">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>10</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B17,'2017-08-14-Geoduck-samples.csv'!C:C,C17,'2017-08-14-Geoduck-samples.csv'!E:E,D17,'2017-08-14-Geoduck-samples.csv'!F:F,E17)</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="3">
+        <f>F17/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="I17" s="2">
+        <v>2</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="M17">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>6</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B18,'2017-08-14-Geoduck-samples.csv'!C:C,C18,'2017-08-14-Geoduck-samples.csv'!E:E,D18,'2017-08-14-Geoduck-samples.csv'!F:F,E18)</f>
+        <v>5</v>
+      </c>
+      <c r="G18" s="3">
+        <f>F18/5</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.2</v>
+      </c>
+      <c r="M18">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>2</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="2">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B19,'2017-08-14-Geoduck-samples.csv'!C:C,C19,'2017-08-14-Geoduck-samples.csv'!E:E,D19,'2017-08-14-Geoduck-samples.csv'!F:F,E19)</f>
+        <v>2</v>
+      </c>
+      <c r="G19" s="3">
+        <f>F19/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="I19" s="2">
+        <v>2</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="M19">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>3</v>
+      </c>
+      <c r="N19" s="3">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="J4" s="8">
-        <v>1</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="N4" s="10">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="O4" s="9">
-        <f t="shared" ref="O4:O21" si="2">N4/15</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B5,'2017-08-14-Geoduck-samples.csv'!C:C,C5,'2017-08-14-Geoduck-samples.csv'!E:E,E5,'2017-08-14-Geoduck-samples.csv'!F:F,F5)</f>
-        <v>4</v>
-      </c>
-      <c r="H5" s="3">
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2">
+        <v>2</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B20,'2017-08-14-Geoduck-samples.csv'!C:C,C20,'2017-08-14-Geoduck-samples.csv'!E:E,D20,'2017-08-14-Geoduck-samples.csv'!F:F,E20)</f>
+        <v>5</v>
+      </c>
+      <c r="G20" s="3">
+        <f>F20/5</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M20">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>10</v>
+      </c>
+      <c r="N20" s="3">
         <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="J5" s="8">
-        <v>1</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="N5" s="10">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="O5" s="9">
-        <f t="shared" si="2"/>
-        <v>0.8666666666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="2">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B6,'2017-08-14-Geoduck-samples.csv'!C:C,C6,'2017-08-14-Geoduck-samples.csv'!E:E,E6,'2017-08-14-Geoduck-samples.csv'!F:F,F6)</f>
-        <v>5</v>
-      </c>
-      <c r="H6" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.93333333333333324</v>
-      </c>
-      <c r="N6" s="10">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="O6" s="9">
-        <f t="shared" si="2"/>
-        <v>0.93333333333333335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B7,'2017-08-14-Geoduck-samples.csv'!C:C,C7,'2017-08-14-Geoduck-samples.csv'!E:E,E7,'2017-08-14-Geoduck-samples.csv'!F:F,F7)</f>
-        <v>3</v>
-      </c>
-      <c r="H7" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B21,'2017-08-14-Geoduck-samples.csv'!C:C,C21,'2017-08-14-Geoduck-samples.csv'!E:E,D21,'2017-08-14-Geoduck-samples.csv'!F:F,E21)</f>
+        <v>3</v>
+      </c>
+      <c r="G21" s="3">
+        <f>F21/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="3">
+        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>0.6</v>
+      </c>
+      <c r="M21">
+        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <v>9</v>
+      </c>
+      <c r="N21" s="3">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="J7" s="8">
-        <v>1</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="N7" s="10">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="O7" s="9">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B8,'2017-08-14-Geoduck-samples.csv'!C:C,C8,'2017-08-14-Geoduck-samples.csv'!E:E,E8,'2017-08-14-Geoduck-samples.csv'!F:F,F8)</f>
-        <v>4</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="J8" s="8">
-        <v>1</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.4</v>
-      </c>
-      <c r="N8" s="10">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="O8" s="9">
-        <f t="shared" si="2"/>
-        <v>0.13333333333333333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="2">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B9,'2017-08-14-Geoduck-samples.csv'!C:C,C9,'2017-08-14-Geoduck-samples.csv'!E:E,E9,'2017-08-14-Geoduck-samples.csv'!F:F,F9)</f>
-        <v>5</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J9" s="8">
-        <v>1</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.73333333333333339</v>
-      </c>
-      <c r="N9" s="10">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="O9" s="9">
-        <f t="shared" si="2"/>
-        <v>0.73333333333333328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="2">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B10,'2017-08-14-Geoduck-samples.csv'!C:C,C10,'2017-08-14-Geoduck-samples.csv'!E:E,E10,'2017-08-14-Geoduck-samples.csv'!F:F,F10)</f>
-        <v>5</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J10" s="8">
-        <v>1</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>1</v>
-      </c>
-      <c r="N10" s="10">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="O10" s="9">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="2">
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B11,'2017-08-14-Geoduck-samples.csv'!C:C,C11,'2017-08-14-Geoduck-samples.csv'!E:E,E11,'2017-08-14-Geoduck-samples.csv'!F:F,F11)</f>
-        <v>5</v>
-      </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J11" s="8">
-        <v>1</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="9">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.93333333333333324</v>
-      </c>
-      <c r="N11" s="10">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="O11" s="9">
-        <f t="shared" si="2"/>
-        <v>0.93333333333333335</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="2">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B12,'2017-08-14-Geoduck-samples.csv'!C:C,C12,'2017-08-14-Geoduck-samples.csv'!E:E,E12,'2017-08-14-Geoduck-samples.csv'!F:F,F12)</f>
-        <v>3</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="J12" s="2">
-        <v>2</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.40000000000000008</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="O12" s="3">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="2">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B13,'2017-08-14-Geoduck-samples.csv'!C:C,C13,'2017-08-14-Geoduck-samples.csv'!E:E,E13,'2017-08-14-Geoduck-samples.csv'!F:F,F13)</f>
-        <v>5</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J13" s="2">
-        <v>2</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.46666666666666662</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="O13" s="3">
-        <f t="shared" si="2"/>
-        <v>0.46666666666666667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="2">
-        <v>5</v>
-      </c>
-      <c r="G14">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B14,'2017-08-14-Geoduck-samples.csv'!C:C,C14,'2017-08-14-Geoduck-samples.csv'!E:E,E14,'2017-08-14-Geoduck-samples.csv'!F:F,F14)</f>
-        <v>4</v>
-      </c>
-      <c r="H14" s="3">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="J14" s="2">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.9</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="O14" s="3">
-        <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="2">
-        <v>6</v>
-      </c>
-      <c r="G15">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B15,'2017-08-14-Geoduck-samples.csv'!C:C,C15,'2017-08-14-Geoduck-samples.csv'!E:E,E15,'2017-08-14-Geoduck-samples.csv'!F:F,F15)</f>
-        <v>5</v>
-      </c>
-      <c r="H15" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J15" s="2">
-        <v>2</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.6</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="O15" s="3">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="2">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B16,'2017-08-14-Geoduck-samples.csv'!C:C,C16,'2017-08-14-Geoduck-samples.csv'!E:E,E16,'2017-08-14-Geoduck-samples.csv'!F:F,F16)</f>
-        <v>3</v>
-      </c>
-      <c r="H16" s="3">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="J16" s="2">
-        <v>2</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="O16" s="3">
-        <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="2">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="2">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B17,'2017-08-14-Geoduck-samples.csv'!C:C,C17,'2017-08-14-Geoduck-samples.csv'!E:E,E17,'2017-08-14-Geoduck-samples.csv'!F:F,F17)</f>
-        <v>4</v>
-      </c>
-      <c r="H17" s="3">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="J17" s="2">
-        <v>2</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="O17" s="3">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="2">
-        <v>2</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="2">
-        <v>3</v>
-      </c>
-      <c r="G18">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B18,'2017-08-14-Geoduck-samples.csv'!C:C,C18,'2017-08-14-Geoduck-samples.csv'!E:E,E18,'2017-08-14-Geoduck-samples.csv'!F:F,F18)</f>
-        <v>5</v>
-      </c>
-      <c r="H18" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J18" s="2">
-        <v>2</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.2</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="O18" s="3">
-        <f t="shared" si="2"/>
-        <v>0.13333333333333333</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="2">
-        <v>6</v>
-      </c>
-      <c r="G19">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B19,'2017-08-14-Geoduck-samples.csv'!C:C,C19,'2017-08-14-Geoduck-samples.csv'!E:E,E19,'2017-08-14-Geoduck-samples.csv'!F:F,F19)</f>
-        <v>2</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="J19" s="2">
-        <v>2</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.20000000000000004</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="O19" s="3">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="2">
-        <v>2</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B20,'2017-08-14-Geoduck-samples.csv'!C:C,C20,'2017-08-14-Geoduck-samples.csv'!E:E,E20,'2017-08-14-Geoduck-samples.csv'!F:F,F20)</f>
-        <v>5</v>
-      </c>
-      <c r="H20" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J20" s="2">
-        <v>2</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M20" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="O20" s="3">
-        <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="2">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="2">
-        <v>2</v>
-      </c>
-      <c r="G21">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B21,'2017-08-14-Geoduck-samples.csv'!C:C,C21,'2017-08-14-Geoduck-samples.csv'!E:E,E21,'2017-08-14-Geoduck-samples.csv'!F:F,F21)</f>
-        <v>3</v>
-      </c>
-      <c r="H21" s="3">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="J21" s="2">
-        <v>2</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M21" s="3">
-        <f>AVERAGEIFS(H:H,B:B,J:J,C:C,K:K,E:E,L:L)</f>
-        <v>0.6</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="O21" s="3">
-        <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="2">
         <v>2</v>
       </c>
@@ -7972,24 +7977,21 @@
         <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="2">
-        <v>3</v>
-      </c>
-      <c r="G22">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B22,'2017-08-14-Geoduck-samples.csv'!C:C,C22,'2017-08-14-Geoduck-samples.csv'!E:E,E22,'2017-08-14-Geoduck-samples.csv'!F:F,F22)</f>
-        <v>3</v>
-      </c>
-      <c r="H22" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B22,'2017-08-14-Geoduck-samples.csv'!C:C,C22,'2017-08-14-Geoduck-samples.csv'!E:E,D22,'2017-08-14-Geoduck-samples.csv'!F:F,E22)</f>
+        <v>3</v>
+      </c>
+      <c r="G22" s="3">
+        <f>F22/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:14">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -8000,24 +8002,21 @@
         <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="2">
-        <v>4</v>
-      </c>
-      <c r="G23">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B23,'2017-08-14-Geoduck-samples.csv'!C:C,C23,'2017-08-14-Geoduck-samples.csv'!E:E,E23,'2017-08-14-Geoduck-samples.csv'!F:F,F23)</f>
+        <v>39</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B23,'2017-08-14-Geoduck-samples.csv'!C:C,C23,'2017-08-14-Geoduck-samples.csv'!E:E,D23,'2017-08-14-Geoduck-samples.csv'!F:F,E23)</f>
         <v>5</v>
       </c>
-      <c r="H23" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="G23" s="3">
+        <f>F23/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -8028,24 +8027,33 @@
         <v>43</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="2">
+        <v>39</v>
+      </c>
+      <c r="E24" s="2">
         <v>5</v>
       </c>
-      <c r="G24">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B24,'2017-08-14-Geoduck-samples.csv'!C:C,C24,'2017-08-14-Geoduck-samples.csv'!E:E,E24,'2017-08-14-Geoduck-samples.csv'!F:F,F24)</f>
+      <c r="F24">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B24,'2017-08-14-Geoduck-samples.csv'!C:C,C24,'2017-08-14-Geoduck-samples.csv'!E:E,D24,'2017-08-14-Geoduck-samples.csv'!F:F,E24)</f>
         <v>5</v>
       </c>
-      <c r="H24" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="G24" s="3">
+        <f>F24/5</f>
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -8056,24 +8064,36 @@
         <v>43</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="2">
+        <v>39</v>
+      </c>
+      <c r="E25" s="2">
         <v>6</v>
       </c>
-      <c r="G25">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B25,'2017-08-14-Geoduck-samples.csv'!C:C,C25,'2017-08-14-Geoduck-samples.csv'!E:E,E25,'2017-08-14-Geoduck-samples.csv'!F:F,F25)</f>
+      <c r="F25">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B25,'2017-08-14-Geoduck-samples.csv'!C:C,C25,'2017-08-14-Geoduck-samples.csv'!E:E,D25,'2017-08-14-Geoduck-samples.csv'!F:F,E25)</f>
         <v>5</v>
       </c>
-      <c r="H25" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="G25" s="3">
+        <f>F25/5</f>
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>254</v>
+      </c>
+      <c r="J25">
+        <v>13</v>
+      </c>
+      <c r="K25">
+        <v>12</v>
+      </c>
+      <c r="L25">
+        <v>10</v>
+      </c>
+      <c r="M25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="2">
         <v>2</v>
       </c>
@@ -8084,24 +8104,36 @@
         <v>43</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B26,'2017-08-14-Geoduck-samples.csv'!C:C,C26,'2017-08-14-Geoduck-samples.csv'!E:E,E26,'2017-08-14-Geoduck-samples.csv'!F:F,F26)</f>
-        <v>4</v>
-      </c>
-      <c r="H26" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B26,'2017-08-14-Geoduck-samples.csv'!C:C,C26,'2017-08-14-Geoduck-samples.csv'!E:E,D26,'2017-08-14-Geoduck-samples.csv'!F:F,E26)</f>
+        <v>4</v>
+      </c>
+      <c r="G26" s="3">
+        <f>F26/5</f>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="I26" t="s">
+        <v>255</v>
+      </c>
+      <c r="J26">
+        <v>12</v>
+      </c>
+      <c r="K26">
+        <v>14</v>
+      </c>
+      <c r="L26">
+        <v>9</v>
+      </c>
+      <c r="M26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="2">
         <v>2</v>
       </c>
@@ -8112,24 +8144,21 @@
         <v>43</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="2">
-        <v>2</v>
-      </c>
-      <c r="G27">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B27,'2017-08-14-Geoduck-samples.csv'!C:C,C27,'2017-08-14-Geoduck-samples.csv'!E:E,E27,'2017-08-14-Geoduck-samples.csv'!F:F,F27)</f>
+        <v>17</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B27,'2017-08-14-Geoduck-samples.csv'!C:C,C27,'2017-08-14-Geoduck-samples.csv'!E:E,D27,'2017-08-14-Geoduck-samples.csv'!F:F,E27)</f>
         <v>5</v>
       </c>
-      <c r="H27" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="G27" s="3">
+        <f>F27/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="2">
         <v>2</v>
       </c>
@@ -8140,24 +8169,21 @@
         <v>43</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="2">
-        <v>3</v>
-      </c>
-      <c r="G28">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B28,'2017-08-14-Geoduck-samples.csv'!C:C,C28,'2017-08-14-Geoduck-samples.csv'!E:E,E28,'2017-08-14-Geoduck-samples.csv'!F:F,F28)</f>
+        <v>17</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B28,'2017-08-14-Geoduck-samples.csv'!C:C,C28,'2017-08-14-Geoduck-samples.csv'!E:E,D28,'2017-08-14-Geoduck-samples.csv'!F:F,E28)</f>
         <v>5</v>
       </c>
-      <c r="H28" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="G28" s="3">
+        <f>F28/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="2">
         <v>3</v>
       </c>
@@ -8168,24 +8194,21 @@
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="2">
-        <v>4</v>
-      </c>
-      <c r="G29">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B29,'2017-08-14-Geoduck-samples.csv'!C:C,C29,'2017-08-14-Geoduck-samples.csv'!E:E,E29,'2017-08-14-Geoduck-samples.csv'!F:F,F29)</f>
-        <v>1</v>
-      </c>
-      <c r="H29" s="3">
-        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B29,'2017-08-14-Geoduck-samples.csv'!C:C,C29,'2017-08-14-Geoduck-samples.csv'!E:E,D29,'2017-08-14-Geoduck-samples.csv'!F:F,E29)</f>
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <f>F29/5</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:14">
       <c r="A30" s="2">
         <v>3</v>
       </c>
@@ -8196,24 +8219,21 @@
         <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="2">
+        <v>39</v>
+      </c>
+      <c r="E30" s="2">
         <v>5</v>
       </c>
-      <c r="G30">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B30,'2017-08-14-Geoduck-samples.csv'!C:C,C30,'2017-08-14-Geoduck-samples.csv'!E:E,E30,'2017-08-14-Geoduck-samples.csv'!F:F,F30)</f>
-        <v>2</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" si="0"/>
+      <c r="F30">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B30,'2017-08-14-Geoduck-samples.csv'!C:C,C30,'2017-08-14-Geoduck-samples.csv'!E:E,D30,'2017-08-14-Geoduck-samples.csv'!F:F,E30)</f>
+        <v>2</v>
+      </c>
+      <c r="G30" s="3">
+        <f>F30/5</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:14">
       <c r="A31" s="2">
         <v>3</v>
       </c>
@@ -8224,24 +8244,21 @@
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="2">
+        <v>39</v>
+      </c>
+      <c r="E31" s="2">
         <v>6</v>
       </c>
-      <c r="G31">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B31,'2017-08-14-Geoduck-samples.csv'!C:C,C31,'2017-08-14-Geoduck-samples.csv'!E:E,E31,'2017-08-14-Geoduck-samples.csv'!F:F,F31)</f>
-        <v>3</v>
-      </c>
-      <c r="H31" s="3">
-        <f t="shared" si="0"/>
+      <c r="F31">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B31,'2017-08-14-Geoduck-samples.csv'!C:C,C31,'2017-08-14-Geoduck-samples.csv'!E:E,D31,'2017-08-14-Geoduck-samples.csv'!F:F,E31)</f>
+        <v>3</v>
+      </c>
+      <c r="G31" s="3">
+        <f>F31/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:14">
       <c r="A32" s="2">
         <v>4</v>
       </c>
@@ -8252,24 +8269,21 @@
         <v>15</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="2">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B32,'2017-08-14-Geoduck-samples.csv'!C:C,C32,'2017-08-14-Geoduck-samples.csv'!E:E,E32,'2017-08-14-Geoduck-samples.csv'!F:F,F32)</f>
-        <v>3</v>
-      </c>
-      <c r="H32" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B32,'2017-08-14-Geoduck-samples.csv'!C:C,C32,'2017-08-14-Geoduck-samples.csv'!E:E,D32,'2017-08-14-Geoduck-samples.csv'!F:F,E32)</f>
+        <v>3</v>
+      </c>
+      <c r="G32" s="3">
+        <f>F32/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
         <v>4</v>
       </c>
@@ -8280,24 +8294,21 @@
         <v>15</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="2">
-        <v>2</v>
-      </c>
-      <c r="G33">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B33,'2017-08-14-Geoduck-samples.csv'!C:C,C33,'2017-08-14-Geoduck-samples.csv'!E:E,E33,'2017-08-14-Geoduck-samples.csv'!F:F,F33)</f>
-        <v>3</v>
-      </c>
-      <c r="H33" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B33,'2017-08-14-Geoduck-samples.csv'!C:C,C33,'2017-08-14-Geoduck-samples.csv'!E:E,D33,'2017-08-14-Geoduck-samples.csv'!F:F,E33)</f>
+        <v>3</v>
+      </c>
+      <c r="G33" s="3">
+        <f>F33/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
         <v>4</v>
       </c>
@@ -8308,24 +8319,21 @@
         <v>15</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="2">
-        <v>3</v>
-      </c>
-      <c r="G34">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B34,'2017-08-14-Geoduck-samples.csv'!C:C,C34,'2017-08-14-Geoduck-samples.csv'!E:E,E34,'2017-08-14-Geoduck-samples.csv'!F:F,F34)</f>
-        <v>1</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B34,'2017-08-14-Geoduck-samples.csv'!C:C,C34,'2017-08-14-Geoduck-samples.csv'!E:E,D34,'2017-08-14-Geoduck-samples.csv'!F:F,E34)</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
+        <f>F34/5</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
         <v>3</v>
       </c>
@@ -8336,24 +8344,21 @@
         <v>38</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" s="2">
-        <v>4</v>
-      </c>
-      <c r="G35">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B35,'2017-08-14-Geoduck-samples.csv'!C:C,C35,'2017-08-14-Geoduck-samples.csv'!E:E,E35,'2017-08-14-Geoduck-samples.csv'!F:F,F35)</f>
+        <v>39</v>
+      </c>
+      <c r="E35" s="2">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B35,'2017-08-14-Geoduck-samples.csv'!C:C,C35,'2017-08-14-Geoduck-samples.csv'!E:E,D35,'2017-08-14-Geoduck-samples.csv'!F:F,E35)</f>
         <v>5</v>
       </c>
-      <c r="H35" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="G35" s="3">
+        <f>F35/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="2">
         <v>3</v>
       </c>
@@ -8364,24 +8369,21 @@
         <v>38</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36" s="2">
+        <v>39</v>
+      </c>
+      <c r="E36" s="2">
         <v>6</v>
       </c>
-      <c r="G36">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B36,'2017-08-14-Geoduck-samples.csv'!C:C,C36,'2017-08-14-Geoduck-samples.csv'!E:E,E36,'2017-08-14-Geoduck-samples.csv'!F:F,F36)</f>
-        <v>4</v>
-      </c>
-      <c r="H36" s="3">
-        <f t="shared" si="0"/>
+      <c r="F36">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B36,'2017-08-14-Geoduck-samples.csv'!C:C,C36,'2017-08-14-Geoduck-samples.csv'!E:E,D36,'2017-08-14-Geoduck-samples.csv'!F:F,E36)</f>
+        <v>4</v>
+      </c>
+      <c r="G36" s="3">
+        <f>F36/5</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:7">
       <c r="A37" s="2">
         <v>4</v>
       </c>
@@ -8392,24 +8394,21 @@
         <v>38</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="2">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B37,'2017-08-14-Geoduck-samples.csv'!C:C,C37,'2017-08-14-Geoduck-samples.csv'!E:E,E37,'2017-08-14-Geoduck-samples.csv'!F:F,F37)</f>
-        <v>3</v>
-      </c>
-      <c r="H37" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B37,'2017-08-14-Geoduck-samples.csv'!C:C,C37,'2017-08-14-Geoduck-samples.csv'!E:E,D37,'2017-08-14-Geoduck-samples.csv'!F:F,E37)</f>
+        <v>3</v>
+      </c>
+      <c r="G37" s="3">
+        <f>F37/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
         <v>4</v>
       </c>
@@ -8420,24 +8419,21 @@
         <v>38</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" s="2">
-        <v>2</v>
-      </c>
-      <c r="G38">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B38,'2017-08-14-Geoduck-samples.csv'!C:C,C38,'2017-08-14-Geoduck-samples.csv'!E:E,E38,'2017-08-14-Geoduck-samples.csv'!F:F,F38)</f>
-        <v>3</v>
-      </c>
-      <c r="H38" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B38,'2017-08-14-Geoduck-samples.csv'!C:C,C38,'2017-08-14-Geoduck-samples.csv'!E:E,D38,'2017-08-14-Geoduck-samples.csv'!F:F,E38)</f>
+        <v>3</v>
+      </c>
+      <c r="G38" s="3">
+        <f>F38/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:7">
       <c r="A39" s="2">
         <v>3</v>
       </c>
@@ -8448,24 +8444,21 @@
         <v>45</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F39" s="2">
-        <v>4</v>
-      </c>
-      <c r="G39">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B39,'2017-08-14-Geoduck-samples.csv'!C:C,C39,'2017-08-14-Geoduck-samples.csv'!E:E,E39,'2017-08-14-Geoduck-samples.csv'!F:F,F39)</f>
+        <v>39</v>
+      </c>
+      <c r="E39" s="2">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B39,'2017-08-14-Geoduck-samples.csv'!C:C,C39,'2017-08-14-Geoduck-samples.csv'!E:E,D39,'2017-08-14-Geoduck-samples.csv'!F:F,E39)</f>
         <v>5</v>
       </c>
-      <c r="H39" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="G39" s="3">
+        <f>F39/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="2">
         <v>3</v>
       </c>
@@ -8476,24 +8469,21 @@
         <v>45</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F40" s="2">
+        <v>39</v>
+      </c>
+      <c r="E40" s="2">
         <v>5</v>
       </c>
-      <c r="G40">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B40,'2017-08-14-Geoduck-samples.csv'!C:C,C40,'2017-08-14-Geoduck-samples.csv'!E:E,E40,'2017-08-14-Geoduck-samples.csv'!F:F,F40)</f>
-        <v>1</v>
-      </c>
-      <c r="H40" s="3">
-        <f t="shared" si="0"/>
+      <c r="F40">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B40,'2017-08-14-Geoduck-samples.csv'!C:C,C40,'2017-08-14-Geoduck-samples.csv'!E:E,D40,'2017-08-14-Geoduck-samples.csv'!F:F,E40)</f>
+        <v>1</v>
+      </c>
+      <c r="G40" s="3">
+        <f>F40/5</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:7">
       <c r="A41" s="2">
         <v>3</v>
       </c>
@@ -8504,24 +8494,21 @@
         <v>45</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F41" s="2">
+        <v>39</v>
+      </c>
+      <c r="E41" s="2">
         <v>6</v>
       </c>
-      <c r="G41">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B41,'2017-08-14-Geoduck-samples.csv'!C:C,C41,'2017-08-14-Geoduck-samples.csv'!E:E,E41,'2017-08-14-Geoduck-samples.csv'!F:F,F41)</f>
-        <v>4</v>
-      </c>
-      <c r="H41" s="3">
-        <f t="shared" si="0"/>
+      <c r="F41">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B41,'2017-08-14-Geoduck-samples.csv'!C:C,C41,'2017-08-14-Geoduck-samples.csv'!E:E,D41,'2017-08-14-Geoduck-samples.csv'!F:F,E41)</f>
+        <v>4</v>
+      </c>
+      <c r="G41" s="3">
+        <f>F41/5</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:7">
       <c r="A42" s="2">
         <v>4</v>
       </c>
@@ -8532,24 +8519,21 @@
         <v>45</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F42" s="2">
-        <v>2</v>
-      </c>
-      <c r="G42">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B42,'2017-08-14-Geoduck-samples.csv'!C:C,C42,'2017-08-14-Geoduck-samples.csv'!E:E,E42,'2017-08-14-Geoduck-samples.csv'!F:F,F42)</f>
-        <v>2</v>
-      </c>
-      <c r="H42" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B42,'2017-08-14-Geoduck-samples.csv'!C:C,C42,'2017-08-14-Geoduck-samples.csv'!E:E,D42,'2017-08-14-Geoduck-samples.csv'!F:F,E42)</f>
+        <v>2</v>
+      </c>
+      <c r="G42" s="3">
+        <f>F42/5</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:7">
       <c r="A43" s="2">
         <v>4</v>
       </c>
@@ -8560,24 +8544,21 @@
         <v>45</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="2">
-        <v>3</v>
-      </c>
-      <c r="G43">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B43,'2017-08-14-Geoduck-samples.csv'!C:C,C43,'2017-08-14-Geoduck-samples.csv'!E:E,E43,'2017-08-14-Geoduck-samples.csv'!F:F,F43)</f>
-        <v>4</v>
-      </c>
-      <c r="H43" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E43" s="2">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B43,'2017-08-14-Geoduck-samples.csv'!C:C,C43,'2017-08-14-Geoduck-samples.csv'!E:E,D43,'2017-08-14-Geoduck-samples.csv'!F:F,E43)</f>
+        <v>4</v>
+      </c>
+      <c r="G43" s="3">
+        <f>F43/5</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:7">
       <c r="A44" s="2">
         <v>4</v>
       </c>
@@ -8588,24 +8569,21 @@
         <v>42</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F44" s="2">
+        <v>39</v>
+      </c>
+      <c r="E44" s="2">
         <v>5</v>
       </c>
-      <c r="G44">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B44,'2017-08-14-Geoduck-samples.csv'!C:C,C44,'2017-08-14-Geoduck-samples.csv'!E:E,E44,'2017-08-14-Geoduck-samples.csv'!F:F,F44)</f>
-        <v>1</v>
-      </c>
-      <c r="H44" s="3">
-        <f t="shared" si="0"/>
+      <c r="F44">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B44,'2017-08-14-Geoduck-samples.csv'!C:C,C44,'2017-08-14-Geoduck-samples.csv'!E:E,D44,'2017-08-14-Geoduck-samples.csv'!F:F,E44)</f>
+        <v>1</v>
+      </c>
+      <c r="G44" s="3">
+        <f>F44/5</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
         <v>4</v>
       </c>
@@ -8616,24 +8594,21 @@
         <v>42</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F45" s="2">
+        <v>39</v>
+      </c>
+      <c r="E45" s="2">
         <v>6</v>
       </c>
-      <c r="G45">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B45,'2017-08-14-Geoduck-samples.csv'!C:C,C45,'2017-08-14-Geoduck-samples.csv'!E:E,E45,'2017-08-14-Geoduck-samples.csv'!F:F,F45)</f>
-        <v>1</v>
-      </c>
-      <c r="H45" s="3">
-        <f t="shared" si="0"/>
+      <c r="F45">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B45,'2017-08-14-Geoduck-samples.csv'!C:C,C45,'2017-08-14-Geoduck-samples.csv'!E:E,D45,'2017-08-14-Geoduck-samples.csv'!F:F,E45)</f>
+        <v>1</v>
+      </c>
+      <c r="G45" s="3">
+        <f>F45/5</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:7">
       <c r="A46" s="2">
         <v>4</v>
       </c>
@@ -8644,24 +8619,21 @@
         <v>42</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F46" s="2">
-        <v>1</v>
-      </c>
-      <c r="G46">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B46,'2017-08-14-Geoduck-samples.csv'!C:C,C46,'2017-08-14-Geoduck-samples.csv'!E:E,E46,'2017-08-14-Geoduck-samples.csv'!F:F,F46)</f>
-        <v>1</v>
-      </c>
-      <c r="H46" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B46,'2017-08-14-Geoduck-samples.csv'!C:C,C46,'2017-08-14-Geoduck-samples.csv'!E:E,D46,'2017-08-14-Geoduck-samples.csv'!F:F,E46)</f>
+        <v>1</v>
+      </c>
+      <c r="G46" s="3">
+        <f>F46/5</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
         <v>4</v>
       </c>
@@ -8672,24 +8644,21 @@
         <v>42</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" s="2">
-        <v>2</v>
-      </c>
-      <c r="G47">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B47,'2017-08-14-Geoduck-samples.csv'!C:C,C47,'2017-08-14-Geoduck-samples.csv'!E:E,E47,'2017-08-14-Geoduck-samples.csv'!F:F,F47)</f>
-        <v>1</v>
-      </c>
-      <c r="H47" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B47,'2017-08-14-Geoduck-samples.csv'!C:C,C47,'2017-08-14-Geoduck-samples.csv'!E:E,D47,'2017-08-14-Geoduck-samples.csv'!F:F,E47)</f>
+        <v>1</v>
+      </c>
+      <c r="G47" s="3">
+        <f>F47/5</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:7">
       <c r="A48" s="2">
         <v>4</v>
       </c>
@@ -8700,24 +8669,21 @@
         <v>42</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" s="2">
-        <v>3</v>
-      </c>
-      <c r="G48">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B48,'2017-08-14-Geoduck-samples.csv'!C:C,C48,'2017-08-14-Geoduck-samples.csv'!E:E,E48,'2017-08-14-Geoduck-samples.csv'!F:F,F48)</f>
-        <v>1</v>
-      </c>
-      <c r="H48" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E48" s="2">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B48,'2017-08-14-Geoduck-samples.csv'!C:C,C48,'2017-08-14-Geoduck-samples.csv'!E:E,D48,'2017-08-14-Geoduck-samples.csv'!F:F,E48)</f>
+        <v>1</v>
+      </c>
+      <c r="G48" s="3">
+        <f>F48/5</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
         <v>3</v>
       </c>
@@ -8728,24 +8694,21 @@
         <v>43</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F49" s="2">
-        <v>4</v>
-      </c>
-      <c r="G49">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B49,'2017-08-14-Geoduck-samples.csv'!C:C,C49,'2017-08-14-Geoduck-samples.csv'!E:E,E49,'2017-08-14-Geoduck-samples.csv'!F:F,F49)</f>
-        <v>3</v>
-      </c>
-      <c r="H49" s="3">
-        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E49" s="2">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B49,'2017-08-14-Geoduck-samples.csv'!C:C,C49,'2017-08-14-Geoduck-samples.csv'!E:E,D49,'2017-08-14-Geoduck-samples.csv'!F:F,E49)</f>
+        <v>3</v>
+      </c>
+      <c r="G49" s="3">
+        <f>F49/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
         <v>3</v>
       </c>
@@ -8756,24 +8719,21 @@
         <v>43</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F50" s="2">
+        <v>39</v>
+      </c>
+      <c r="E50" s="2">
         <v>5</v>
       </c>
-      <c r="G50">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B50,'2017-08-14-Geoduck-samples.csv'!C:C,C50,'2017-08-14-Geoduck-samples.csv'!E:E,E50,'2017-08-14-Geoduck-samples.csv'!F:F,F50)</f>
-        <v>4</v>
-      </c>
-      <c r="H50" s="3">
-        <f t="shared" si="0"/>
+      <c r="F50">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B50,'2017-08-14-Geoduck-samples.csv'!C:C,C50,'2017-08-14-Geoduck-samples.csv'!E:E,D50,'2017-08-14-Geoduck-samples.csv'!F:F,E50)</f>
+        <v>4</v>
+      </c>
+      <c r="G50" s="3">
+        <f>F50/5</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
         <v>3</v>
       </c>
@@ -8784,24 +8744,21 @@
         <v>43</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F51" s="2">
+        <v>39</v>
+      </c>
+      <c r="E51" s="2">
         <v>6</v>
       </c>
-      <c r="G51">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B51,'2017-08-14-Geoduck-samples.csv'!C:C,C51,'2017-08-14-Geoduck-samples.csv'!E:E,E51,'2017-08-14-Geoduck-samples.csv'!F:F,F51)</f>
-        <v>3</v>
-      </c>
-      <c r="H51" s="3">
-        <f t="shared" si="0"/>
+      <c r="F51">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B51,'2017-08-14-Geoduck-samples.csv'!C:C,C51,'2017-08-14-Geoduck-samples.csv'!E:E,D51,'2017-08-14-Geoduck-samples.csv'!F:F,E51)</f>
+        <v>3</v>
+      </c>
+      <c r="G51" s="3">
+        <f>F51/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
         <v>4</v>
       </c>
@@ -8812,24 +8769,21 @@
         <v>43</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F52" s="2">
-        <v>1</v>
-      </c>
-      <c r="G52">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B52,'2017-08-14-Geoduck-samples.csv'!C:C,C52,'2017-08-14-Geoduck-samples.csv'!E:E,E52,'2017-08-14-Geoduck-samples.csv'!F:F,F52)</f>
-        <v>2</v>
-      </c>
-      <c r="H52" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E52" s="2">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B52,'2017-08-14-Geoduck-samples.csv'!C:C,C52,'2017-08-14-Geoduck-samples.csv'!E:E,D52,'2017-08-14-Geoduck-samples.csv'!F:F,E52)</f>
+        <v>2</v>
+      </c>
+      <c r="G52" s="3">
+        <f>F52/5</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:7">
       <c r="A53" s="2">
         <v>4</v>
       </c>
@@ -8840,24 +8794,21 @@
         <v>43</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F53" s="2">
-        <v>2</v>
-      </c>
-      <c r="G53">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B53,'2017-08-14-Geoduck-samples.csv'!C:C,C53,'2017-08-14-Geoduck-samples.csv'!E:E,E53,'2017-08-14-Geoduck-samples.csv'!F:F,F53)</f>
-        <v>3</v>
-      </c>
-      <c r="H53" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E53" s="2">
+        <v>2</v>
+      </c>
+      <c r="F53">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B53,'2017-08-14-Geoduck-samples.csv'!C:C,C53,'2017-08-14-Geoduck-samples.csv'!E:E,D53,'2017-08-14-Geoduck-samples.csv'!F:F,E53)</f>
+        <v>3</v>
+      </c>
+      <c r="G53" s="3">
+        <f>F53/5</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:7">
       <c r="A54" s="2">
         <v>4</v>
       </c>
@@ -8868,34 +8819,31 @@
         <v>43</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F54" s="2">
-        <v>3</v>
-      </c>
-      <c r="G54">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B54,'2017-08-14-Geoduck-samples.csv'!C:C,C54,'2017-08-14-Geoduck-samples.csv'!E:E,E54,'2017-08-14-Geoduck-samples.csv'!F:F,F54)</f>
-        <v>4</v>
-      </c>
-      <c r="H54" s="3">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E54" s="2">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B54,'2017-08-14-Geoduck-samples.csv'!C:C,C54,'2017-08-14-Geoduck-samples.csv'!E:E,D54,'2017-08-14-Geoduck-samples.csv'!F:F,E54)</f>
+        <v>4</v>
+      </c>
+      <c r="G54" s="3">
+        <f>F54/5</f>
         <v>0.8</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F54">
+  <sortState ref="A2:G54">
     <sortCondition ref="B2:B54"/>
     <sortCondition ref="C2:C54"/>
+    <sortCondition ref="D2:D54"/>
     <sortCondition ref="E2:E54"/>
-    <sortCondition ref="F2:F54"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="M3:M21 N2:N21" emptyCellReference="1"/>
+    <ignoredError sqref="L3:L21 M2:M21" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -8903,4 +8851,621 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A2,'2017-08-14-Geoduck-samples.csv'!C:C,B2,'2017-08-14-Geoduck-samples.csv'!E:E,C2,'2017-08-14-Geoduck-samples.csv'!F:F,E2)</f>
+        <v>4</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A3,'2017-08-14-Geoduck-samples.csv'!C:C,B3,'2017-08-14-Geoduck-samples.csv'!E:E,C3,'2017-08-14-Geoduck-samples.csv'!F:F,E3)</f>
+        <v>5</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A4,'2017-08-14-Geoduck-samples.csv'!C:C,B4,'2017-08-14-Geoduck-samples.csv'!E:E,C4,'2017-08-14-Geoduck-samples.csv'!F:F,E4)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <f>F4/5</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A5,'2017-08-14-Geoduck-samples.csv'!C:C,B5,'2017-08-14-Geoduck-samples.csv'!E:E,C5,'2017-08-14-Geoduck-samples.csv'!F:F,E5)</f>
+        <v>4</v>
+      </c>
+      <c r="G5" s="3">
+        <f>F5/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A6,'2017-08-14-Geoduck-samples.csv'!C:C,B6,'2017-08-14-Geoduck-samples.csv'!E:E,C6,'2017-08-14-Geoduck-samples.csv'!F:F,E6)</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="3">
+        <f>F6/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A7,'2017-08-14-Geoduck-samples.csv'!C:C,B7,'2017-08-14-Geoduck-samples.csv'!E:E,C7,'2017-08-14-Geoduck-samples.csv'!F:F,E7)</f>
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <f>F7/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A8,'2017-08-14-Geoduck-samples.csv'!C:C,B8,'2017-08-14-Geoduck-samples.csv'!E:E,C8,'2017-08-14-Geoduck-samples.csv'!F:F,E8)</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <f>F8/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A9,'2017-08-14-Geoduck-samples.csv'!C:C,B9,'2017-08-14-Geoduck-samples.csv'!E:E,C9,'2017-08-14-Geoduck-samples.csv'!F:F,E9)</f>
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
+        <f>F9/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A10,'2017-08-14-Geoduck-samples.csv'!C:C,B10,'2017-08-14-Geoduck-samples.csv'!E:E,C10,'2017-08-14-Geoduck-samples.csv'!F:F,E10)</f>
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <f>F10/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A11,'2017-08-14-Geoduck-samples.csv'!C:C,B11,'2017-08-14-Geoduck-samples.csv'!E:E,C11,'2017-08-14-Geoduck-samples.csv'!F:F,E11)</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="3">
+        <f>F11/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A12,'2017-08-14-Geoduck-samples.csv'!C:C,B12,'2017-08-14-Geoduck-samples.csv'!E:E,C12,'2017-08-14-Geoduck-samples.csv'!F:F,E12)</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
+        <f>F12/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A13,'2017-08-14-Geoduck-samples.csv'!C:C,B13,'2017-08-14-Geoduck-samples.csv'!E:E,C13,'2017-08-14-Geoduck-samples.csv'!F:F,E13)</f>
+        <v>5</v>
+      </c>
+      <c r="G13" s="3">
+        <f>F13/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A14,'2017-08-14-Geoduck-samples.csv'!C:C,B14,'2017-08-14-Geoduck-samples.csv'!E:E,C14,'2017-08-14-Geoduck-samples.csv'!F:F,E14)</f>
+        <v>4</v>
+      </c>
+      <c r="G14" s="3">
+        <f>F14/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A15,'2017-08-14-Geoduck-samples.csv'!C:C,B15,'2017-08-14-Geoduck-samples.csv'!E:E,C15,'2017-08-14-Geoduck-samples.csv'!F:F,E15)</f>
+        <v>5</v>
+      </c>
+      <c r="G15" s="3">
+        <f>F15/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A16,'2017-08-14-Geoduck-samples.csv'!C:C,B16,'2017-08-14-Geoduck-samples.csv'!E:E,C16,'2017-08-14-Geoduck-samples.csv'!F:F,E16)</f>
+        <v>3</v>
+      </c>
+      <c r="G16" s="3">
+        <f>F16/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A17,'2017-08-14-Geoduck-samples.csv'!C:C,B17,'2017-08-14-Geoduck-samples.csv'!E:E,C17,'2017-08-14-Geoduck-samples.csv'!F:F,E17)</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="3">
+        <f>F17/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A18,'2017-08-14-Geoduck-samples.csv'!C:C,B18,'2017-08-14-Geoduck-samples.csv'!E:E,C18,'2017-08-14-Geoduck-samples.csv'!F:F,E18)</f>
+        <v>5</v>
+      </c>
+      <c r="G18" s="3">
+        <f>F18/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E19" s="2">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A19,'2017-08-14-Geoduck-samples.csv'!C:C,B19,'2017-08-14-Geoduck-samples.csv'!E:E,C19,'2017-08-14-Geoduck-samples.csv'!F:F,E19)</f>
+        <v>5</v>
+      </c>
+      <c r="G19" s="3">
+        <f>F19/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A20,'2017-08-14-Geoduck-samples.csv'!C:C,B20,'2017-08-14-Geoduck-samples.csv'!E:E,C20,'2017-08-14-Geoduck-samples.csv'!F:F,E20)</f>
+        <v>5</v>
+      </c>
+      <c r="G20" s="3">
+        <f>F20/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E21" s="2">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A21,'2017-08-14-Geoduck-samples.csv'!C:C,B21,'2017-08-14-Geoduck-samples.csv'!E:E,C21,'2017-08-14-Geoduck-samples.csv'!F:F,E21)</f>
+        <v>5</v>
+      </c>
+      <c r="G21" s="3">
+        <f>F21/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A22,'2017-08-14-Geoduck-samples.csv'!C:C,B22,'2017-08-14-Geoduck-samples.csv'!E:E,C22,'2017-08-14-Geoduck-samples.csv'!F:F,E22)</f>
+        <v>4</v>
+      </c>
+      <c r="G22" s="3">
+        <f>F22/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A23,'2017-08-14-Geoduck-samples.csv'!C:C,B23,'2017-08-14-Geoduck-samples.csv'!E:E,C23,'2017-08-14-Geoduck-samples.csv'!F:F,E23)</f>
+        <v>5</v>
+      </c>
+      <c r="G23" s="3">
+        <f>F23/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A24,'2017-08-14-Geoduck-samples.csv'!C:C,B24,'2017-08-14-Geoduck-samples.csv'!E:E,C24,'2017-08-14-Geoduck-samples.csv'!F:F,E24)</f>
+        <v>5</v>
+      </c>
+      <c r="G24" s="3">
+        <f>F24/5</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
lots of env. data updates, presentation for NSA
</commit_message>
<xml_diff>
--- a/data/Survival-stats.xlsx
+++ b/data/Survival-stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28331"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="0" windowWidth="16900" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8700" yWindow="0" windowWidth="16900" windowHeight="15460" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2017-08-14-Geoduck-samples.csv" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="256">
   <si>
     <t>Box #</t>
   </si>
@@ -1323,7 +1323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W183"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" workbookViewId="0">
+    <sheetView topLeftCell="A80" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:H21"/>
     </sheetView>
   </sheetViews>
@@ -6993,8 +6993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24:M26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7067,7 +7067,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="3">
-        <f>F2/5</f>
+        <f t="shared" ref="G2:G33" si="0">F2/5</f>
         <v>0.8</v>
       </c>
       <c r="I2" s="8">
@@ -7080,11 +7080,11 @@
         <v>39</v>
       </c>
       <c r="L2" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" ref="L2:L21" si="1">AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
         <v>0.9</v>
       </c>
       <c r="M2" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" ref="M2:M21" si="2">SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
         <v>9</v>
       </c>
       <c r="N2" s="9">
@@ -7113,7 +7113,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="3">
-        <f>F3/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I3" s="8">
@@ -7126,11 +7126,11 @@
         <v>17</v>
       </c>
       <c r="L3" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="M3" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="N3" s="9">
@@ -7159,7 +7159,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="3">
-        <f>F4/5</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="I4" s="8">
@@ -7172,15 +7172,15 @@
         <v>39</v>
       </c>
       <c r="L4" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="M4" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="N4" s="9">
-        <f t="shared" ref="N4:N21" si="0">M4/15</f>
+        <f t="shared" ref="N4:N21" si="3">M4/15</f>
         <v>0.8</v>
       </c>
     </row>
@@ -7205,7 +7205,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="3">
-        <f>F5/5</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="I5" s="8">
@@ -7218,15 +7218,15 @@
         <v>17</v>
       </c>
       <c r="L5" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.8666666666666667</v>
       </c>
       <c r="M5" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="N5" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.8666666666666667</v>
       </c>
     </row>
@@ -7251,7 +7251,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="3">
-        <f>F6/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I6" s="8">
@@ -7264,15 +7264,15 @@
         <v>39</v>
       </c>
       <c r="L6" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.93333333333333324</v>
       </c>
       <c r="M6" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="N6" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.93333333333333335</v>
       </c>
     </row>
@@ -7297,7 +7297,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="3">
-        <f>F7/5</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="I7" s="8">
@@ -7310,42 +7310,42 @@
         <v>17</v>
       </c>
       <c r="L7" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="M7" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="N7" s="9">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B8,'2017-08-14-Geoduck-samples.csv'!C:C,C8,'2017-08-14-Geoduck-samples.csv'!E:E,D8,'2017-08-14-Geoduck-samples.csv'!F:F,E8)</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,B8,'2017-08-14-Geoduck-samples.csv'!C:C,C8,'2017-08-14-Geoduck-samples.csv'!E:E,D8,'2017-08-14-Geoduck-samples.csv'!F:F,E8)</f>
-        <v>4</v>
-      </c>
-      <c r="G8" s="3">
-        <f>F8/5</f>
-        <v>0.8</v>
-      </c>
       <c r="I8" s="8">
         <v>1</v>
       </c>
@@ -7356,15 +7356,15 @@
         <v>39</v>
       </c>
       <c r="L8" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="M8" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="N8" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.13333333333333333</v>
       </c>
     </row>
@@ -7389,7 +7389,7 @@
         <v>5</v>
       </c>
       <c r="G9" s="3">
-        <f>F9/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I9" s="8">
@@ -7402,15 +7402,15 @@
         <v>17</v>
       </c>
       <c r="L9" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.73333333333333339</v>
       </c>
       <c r="M9" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="N9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.73333333333333328</v>
       </c>
     </row>
@@ -7435,7 +7435,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="3">
-        <f>F10/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I10" s="8">
@@ -7448,15 +7448,15 @@
         <v>39</v>
       </c>
       <c r="L10" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M10" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="N10" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7481,7 +7481,7 @@
         <v>5</v>
       </c>
       <c r="G11" s="3">
-        <f>F11/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I11" s="8">
@@ -7494,15 +7494,15 @@
         <v>17</v>
       </c>
       <c r="L11" s="9">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.93333333333333324</v>
       </c>
       <c r="M11" s="10">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="N11" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.93333333333333335</v>
       </c>
     </row>
@@ -7527,7 +7527,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="3">
-        <f>F12/5</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="I12" s="2">
@@ -7540,15 +7540,15 @@
         <v>39</v>
       </c>
       <c r="L12" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.40000000000000008</v>
       </c>
       <c r="M12">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
     </row>
@@ -7573,7 +7573,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="3">
-        <f>F13/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I13" s="2">
@@ -7586,15 +7586,15 @@
         <v>17</v>
       </c>
       <c r="L13" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.46666666666666662</v>
       </c>
       <c r="M13">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="N13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.46666666666666667</v>
       </c>
     </row>
@@ -7619,7 +7619,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="3">
-        <f>F14/5</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="I14" s="2">
@@ -7632,15 +7632,15 @@
         <v>39</v>
       </c>
       <c r="L14" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
       <c r="M14">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="N14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -7665,7 +7665,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="3">
-        <f>F15/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I15" s="2">
@@ -7678,15 +7678,15 @@
         <v>17</v>
       </c>
       <c r="L15" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="M15">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
     </row>
@@ -7711,7 +7711,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="3">
-        <f>F16/5</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="I16" s="2">
@@ -7724,15 +7724,15 @@
         <v>39</v>
       </c>
       <c r="L16" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="M16">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -7757,7 +7757,7 @@
         <v>4</v>
       </c>
       <c r="G17" s="3">
-        <f>F17/5</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="I17" s="2">
@@ -7770,15 +7770,15 @@
         <v>17</v>
       </c>
       <c r="L17" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="M17">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="N17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
     </row>
@@ -7803,7 +7803,7 @@
         <v>5</v>
       </c>
       <c r="G18" s="3">
-        <f>F18/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I18" s="2">
@@ -7816,15 +7816,15 @@
         <v>39</v>
       </c>
       <c r="L18" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="M18">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="N18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.13333333333333333</v>
       </c>
     </row>
@@ -7849,7 +7849,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="3">
-        <f>F19/5</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="I19" s="2">
@@ -7862,15 +7862,15 @@
         <v>17</v>
       </c>
       <c r="L19" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.20000000000000004</v>
       </c>
       <c r="M19">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
@@ -7895,7 +7895,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="3">
-        <f>F20/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I20" s="2">
@@ -7908,15 +7908,15 @@
         <v>39</v>
       </c>
       <c r="L20" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="M20">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="N20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -7941,7 +7941,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="3">
-        <f>F21/5</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="I21" s="2">
@@ -7954,15 +7954,15 @@
         <v>17</v>
       </c>
       <c r="L21" s="3">
-        <f>AVERAGEIFS(G:G,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="M21">
-        <f>SUMIFS(F:F,B:B,I:I,C:C,J:J,D:D,K:K)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="N21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
     </row>
@@ -7987,7 +7987,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="3">
-        <f>F22/5</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8012,7 +8012,7 @@
         <v>5</v>
       </c>
       <c r="G23" s="3">
-        <f>F23/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -8037,7 +8037,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="3">
-        <f>F24/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J24" s="2" t="s">
@@ -8074,7 +8074,7 @@
         <v>5</v>
       </c>
       <c r="G25" s="3">
-        <f>F25/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I25" t="s">
@@ -8114,7 +8114,7 @@
         <v>4</v>
       </c>
       <c r="G26" s="3">
-        <f>F26/5</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="I26" t="s">
@@ -8154,7 +8154,7 @@
         <v>5</v>
       </c>
       <c r="G27" s="3">
-        <f>F27/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -8179,7 +8179,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="3">
-        <f>F28/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -8204,7 +8204,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="3">
-        <f>F29/5</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -8229,7 +8229,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="3">
-        <f>F30/5</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -8254,7 +8254,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="3">
-        <f>F31/5</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8279,7 +8279,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="3">
-        <f>F32/5</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8304,7 +8304,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="3">
-        <f>F33/5</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8329,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="3">
-        <f>F34/5</f>
+        <f t="shared" ref="G34:G65" si="4">F34/5</f>
         <v>0.2</v>
       </c>
     </row>
@@ -8354,7 +8354,7 @@
         <v>5</v>
       </c>
       <c r="G35" s="3">
-        <f>F35/5</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8379,7 +8379,7 @@
         <v>4</v>
       </c>
       <c r="G36" s="3">
-        <f>F36/5</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
     </row>
@@ -8404,7 +8404,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="3">
-        <f>F37/5</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8429,7 +8429,7 @@
         <v>3</v>
       </c>
       <c r="G38" s="3">
-        <f>F38/5</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8454,7 +8454,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="3">
-        <f>F39/5</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8479,7 +8479,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="3">
-        <f>F40/5</f>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
     </row>
@@ -8504,7 +8504,7 @@
         <v>4</v>
       </c>
       <c r="G41" s="3">
-        <f>F41/5</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
     </row>
@@ -8529,7 +8529,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="3">
-        <f>F42/5</f>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
     </row>
@@ -8554,7 +8554,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="3">
-        <f>F43/5</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
     </row>
@@ -8579,7 +8579,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="3">
-        <f>F44/5</f>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
     </row>
@@ -8604,7 +8604,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="3">
-        <f>F45/5</f>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
     </row>
@@ -8629,7 +8629,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="3">
-        <f>F46/5</f>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
     </row>
@@ -8654,7 +8654,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="3">
-        <f>F47/5</f>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
     </row>
@@ -8679,7 +8679,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="3">
-        <f>F48/5</f>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
     </row>
@@ -8704,7 +8704,7 @@
         <v>3</v>
       </c>
       <c r="G49" s="3">
-        <f>F49/5</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8729,7 +8729,7 @@
         <v>4</v>
       </c>
       <c r="G50" s="3">
-        <f>F50/5</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
     </row>
@@ -8754,7 +8754,7 @@
         <v>3</v>
       </c>
       <c r="G51" s="3">
-        <f>F51/5</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8779,7 +8779,7 @@
         <v>2</v>
       </c>
       <c r="G52" s="3">
-        <f>F52/5</f>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
     </row>
@@ -8804,7 +8804,7 @@
         <v>3</v>
       </c>
       <c r="G53" s="3">
-        <f>F53/5</f>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
     </row>
@@ -8829,7 +8829,7 @@
         <v>4</v>
       </c>
       <c r="G54" s="3">
-        <f>F54/5</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
     </row>
@@ -8855,10 +8855,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8905,7 +8905,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="3">
-        <f>F2/5</f>
+        <f t="shared" ref="G2:G25" si="0">F2/5</f>
         <v>0.8</v>
       </c>
     </row>
@@ -8930,7 +8930,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="3">
-        <f>F3/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -8942,21 +8942,19 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A4,'2017-08-14-Geoduck-samples.csv'!C:C,B4,'2017-08-14-Geoduck-samples.csv'!E:E,C4,'2017-08-14-Geoduck-samples.csv'!F:F,E4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
-        <f>F4/5</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -8973,15 +8971,15 @@
         <v>249</v>
       </c>
       <c r="E5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A5,'2017-08-14-Geoduck-samples.csv'!C:C,B5,'2017-08-14-Geoduck-samples.csv'!E:E,C5,'2017-08-14-Geoduck-samples.csv'!F:F,E5)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" s="3">
-        <f>F5/5</f>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -8998,15 +8996,15 @@
         <v>249</v>
       </c>
       <c r="E6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A6,'2017-08-14-Geoduck-samples.csv'!C:C,B6,'2017-08-14-Geoduck-samples.csv'!E:E,C6,'2017-08-14-Geoduck-samples.csv'!F:F,E6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" s="3">
-        <f>F6/5</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -9014,24 +9012,24 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A7,'2017-08-14-Geoduck-samples.csv'!C:C,B7,'2017-08-14-Geoduck-samples.csv'!E:E,C7,'2017-08-14-Geoduck-samples.csv'!F:F,E7)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G7" s="3">
-        <f>F7/5</f>
-        <v>0.6</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -9048,15 +9046,15 @@
         <v>250</v>
       </c>
       <c r="E8" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A8,'2017-08-14-Geoduck-samples.csv'!C:C,B8,'2017-08-14-Geoduck-samples.csv'!E:E,C8,'2017-08-14-Geoduck-samples.csv'!F:F,E8)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="3">
-        <f>F8/5</f>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -9073,15 +9071,15 @@
         <v>250</v>
       </c>
       <c r="E9" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A9,'2017-08-14-Geoduck-samples.csv'!C:C,B9,'2017-08-14-Geoduck-samples.csv'!E:E,C9,'2017-08-14-Geoduck-samples.csv'!F:F,E9)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="3">
-        <f>F9/5</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -9092,20 +9090,20 @@
         <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F10">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A10,'2017-08-14-Geoduck-samples.csv'!C:C,B10,'2017-08-14-Geoduck-samples.csv'!E:E,C10,'2017-08-14-Geoduck-samples.csv'!F:F,E10)</f>
         <v>5</v>
       </c>
       <c r="G10" s="3">
-        <f>F10/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -9123,14 +9121,14 @@
         <v>251</v>
       </c>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A11,'2017-08-14-Geoduck-samples.csv'!C:C,B11,'2017-08-14-Geoduck-samples.csv'!E:E,C11,'2017-08-14-Geoduck-samples.csv'!F:F,E11)</f>
         <v>5</v>
       </c>
       <c r="G11" s="3">
-        <f>F11/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -9148,15 +9146,15 @@
         <v>251</v>
       </c>
       <c r="E12" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A12,'2017-08-14-Geoduck-samples.csv'!C:C,B12,'2017-08-14-Geoduck-samples.csv'!E:E,C12,'2017-08-14-Geoduck-samples.csv'!F:F,E12)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G12" s="3">
-        <f>F12/5</f>
-        <v>0.6</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -9164,24 +9162,24 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E13" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A13,'2017-08-14-Geoduck-samples.csv'!C:C,B13,'2017-08-14-Geoduck-samples.csv'!E:E,C13,'2017-08-14-Geoduck-samples.csv'!F:F,E13)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G13" s="3">
-        <f>F13/5</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -9198,15 +9196,15 @@
         <v>252</v>
       </c>
       <c r="E14" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A14,'2017-08-14-Geoduck-samples.csv'!C:C,B14,'2017-08-14-Geoduck-samples.csv'!E:E,C14,'2017-08-14-Geoduck-samples.csv'!F:F,E14)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14" s="3">
-        <f>F14/5</f>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -9223,15 +9221,15 @@
         <v>252</v>
       </c>
       <c r="E15" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A15,'2017-08-14-Geoduck-samples.csv'!C:C,B15,'2017-08-14-Geoduck-samples.csv'!E:E,C15,'2017-08-14-Geoduck-samples.csv'!F:F,E15)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G15" s="3">
-        <f>F15/5</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -9242,21 +9240,21 @@
         <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E16" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F16">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A16,'2017-08-14-Geoduck-samples.csv'!C:C,B16,'2017-08-14-Geoduck-samples.csv'!E:E,C16,'2017-08-14-Geoduck-samples.csv'!F:F,E16)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G16" s="3">
-        <f>F16/5</f>
-        <v>0.6</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -9273,15 +9271,15 @@
         <v>253</v>
       </c>
       <c r="E17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A17,'2017-08-14-Geoduck-samples.csv'!C:C,B17,'2017-08-14-Geoduck-samples.csv'!E:E,C17,'2017-08-14-Geoduck-samples.csv'!F:F,E17)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" s="3">
-        <f>F17/5</f>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -9298,15 +9296,15 @@
         <v>253</v>
       </c>
       <c r="E18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A18,'2017-08-14-Geoduck-samples.csv'!C:C,B18,'2017-08-14-Geoduck-samples.csv'!E:E,C18,'2017-08-14-Geoduck-samples.csv'!F:F,E18)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="3">
-        <f>F18/5</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -9314,23 +9312,23 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="E19" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A19,'2017-08-14-Geoduck-samples.csv'!C:C,B19,'2017-08-14-Geoduck-samples.csv'!E:E,C19,'2017-08-14-Geoduck-samples.csv'!F:F,E19)</f>
         <v>5</v>
       </c>
       <c r="G19" s="3">
-        <f>F19/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -9348,14 +9346,14 @@
         <v>247</v>
       </c>
       <c r="E20" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A20,'2017-08-14-Geoduck-samples.csv'!C:C,B20,'2017-08-14-Geoduck-samples.csv'!E:E,C20,'2017-08-14-Geoduck-samples.csv'!F:F,E20)</f>
         <v>5</v>
       </c>
       <c r="G20" s="3">
-        <f>F20/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -9373,14 +9371,14 @@
         <v>247</v>
       </c>
       <c r="E21" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A21,'2017-08-14-Geoduck-samples.csv'!C:C,B21,'2017-08-14-Geoduck-samples.csv'!E:E,C21,'2017-08-14-Geoduck-samples.csv'!F:F,E21)</f>
         <v>5</v>
       </c>
       <c r="G21" s="3">
-        <f>F21/5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -9392,21 +9390,21 @@
         <v>43</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>247</v>
       </c>
       <c r="E22" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F22">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A22,'2017-08-14-Geoduck-samples.csv'!C:C,B22,'2017-08-14-Geoduck-samples.csv'!E:E,C22,'2017-08-14-Geoduck-samples.csv'!F:F,E22)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G22" s="3">
-        <f>F22/5</f>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -9423,15 +9421,15 @@
         <v>247</v>
       </c>
       <c r="E23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A23,'2017-08-14-Geoduck-samples.csv'!C:C,B23,'2017-08-14-Geoduck-samples.csv'!E:E,C23,'2017-08-14-Geoduck-samples.csv'!F:F,E23)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23" s="3">
-        <f>F23/5</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -9448,14 +9446,39 @@
         <v>247</v>
       </c>
       <c r="E24" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24">
         <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A24,'2017-08-14-Geoduck-samples.csv'!C:C,B24,'2017-08-14-Geoduck-samples.csv'!E:E,C24,'2017-08-14-Geoduck-samples.csv'!F:F,E24)</f>
         <v>5</v>
       </c>
       <c r="G24" s="3">
-        <f>F24/5</f>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <f>COUNTIFS('2017-08-14-Geoduck-samples.csv'!B:B,A25,'2017-08-14-Geoduck-samples.csv'!C:C,B25,'2017-08-14-Geoduck-samples.csv'!E:E,C25,'2017-08-14-Geoduck-samples.csv'!F:F,E25)</f>
+        <v>5</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>